<commit_message>
Update MS 365 pages
</commit_message>
<xml_diff>
--- a/Spreadsheet Applications/Analyzing Data with Pie Charts, Line Charts, and What-IF Analysis Tools/Enterprise Fund.xlsx
+++ b/Spreadsheet Applications/Analyzing Data with Pie Charts, Line Charts, and What-IF Analysis Tools/Enterprise Fund.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f3e3711e514002e0/Documents/Personal/Website/Soumya's Website/Spreadsheet Applications/Analyzing Data with Pie Charts^J Line Charts^J and What-IF Analysis Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="11_F7ED7B8641F88DCEDB1BD5F928FCFB673056F833" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CEF13B4-D94D-48AD-8F54-BECD192DBAB3}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="11_F7ED7B8641F88DCEDB1BD5F928FCFB673056F833" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73343FC5-7803-4EFC-B211-6BFF537BEB77}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enterprise Fund Expenditures" sheetId="1" r:id="rId1"/>
@@ -731,6 +731,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -738,7 +739,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -1656,7 +1656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1815,6 +1815,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;F</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>